<commit_message>
Update socket and realtime functionality
server.js
</commit_message>
<xml_diff>
--- a/storage/app/templates/EmployeeListSummary.xlsx
+++ b/storage/app/templates/EmployeeListSummary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;₱&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +109,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -145,14 +153,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -168,6 +170,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -175,18 +201,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -521,91 +535,91 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="11" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>